<commit_message>
fix row 2 short header validation
</commit_message>
<xml_diff>
--- a/api/src/test/resources/sheets/correctShortHeader.xlsx
+++ b/api/src/test/resources/sheets/correctShortHeader.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Source\repos\nrmn-application\api\src\test\resources\sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63AA684F-8B89-437D-A67D-78AC9C2238EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF436CB-BCF2-47E0-A2B1-59463F77AADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29490" yWindow="690" windowWidth="21600" windowHeight="12885" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="-60" windowWidth="28920" windowHeight="17670" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" state="hidden" r:id="rId1"/>
@@ -34,10 +34,9 @@
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="4" r:id="rId10"/>
+    <pivotCache cacheId="5" r:id="rId11"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -6881,7 +6880,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -7000,6 +6999,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -7673,7 +7677,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
@@ -7960,6 +7964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11896,7 +11901,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" itemPrintTitles="1" indent="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" itemPrintTitles="1" indent="0" compact="0" compactData="0">
   <location ref="A3:F28" firstHeaderRow="1" firstDataRow="4" firstDataCol="2"/>
   <pivotFields count="18">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -11991,7 +11996,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0700-000000000000}" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" itemPrintTitles="1" indent="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0700-000000000000}" name="DataPilot1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" itemPrintTitles="1" indent="0" compact="0" compactData="0">
   <location ref="A3:I13" firstHeaderRow="1" firstDataRow="2" firstDataCol="6"/>
   <pivotFields count="60">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -12829,10 +12834,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH1" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="BM15" sqref="BM15"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2:AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75"/>
@@ -13124,89 +13129,89 @@
         <f>SUM(T3:T9999)</f>
         <v>1</v>
       </c>
-      <c r="U2" s="70">
-        <v>0.5</v>
-      </c>
-      <c r="V2" s="70">
+      <c r="U2" s="161">
         <v>1</v>
       </c>
-      <c r="W2" s="70">
-        <v>1.5</v>
-      </c>
-      <c r="X2" s="70">
+      <c r="V2" s="161">
         <v>2</v>
       </c>
-      <c r="Y2" s="70">
-        <v>2.5</v>
-      </c>
-      <c r="Z2" s="70">
+      <c r="W2" s="161">
         <v>3</v>
       </c>
-      <c r="AA2" s="70">
-        <v>3.5</v>
-      </c>
-      <c r="AB2" s="70">
+      <c r="X2" s="161">
         <v>4</v>
       </c>
-      <c r="AC2" s="70">
-        <v>4.5</v>
-      </c>
-      <c r="AD2" s="70">
+      <c r="Y2" s="161">
         <v>5</v>
       </c>
-      <c r="AE2" s="70">
-        <v>5.5</v>
-      </c>
-      <c r="AF2" s="70">
+      <c r="Z2" s="161">
         <v>6</v>
       </c>
-      <c r="AG2" s="70">
-        <v>6.5</v>
-      </c>
-      <c r="AH2" s="70">
-        <v>7</v>
-      </c>
-      <c r="AI2" s="70">
-        <v>7.5</v>
-      </c>
-      <c r="AJ2" s="70">
+      <c r="AA2" s="161">
         <v>8</v>
       </c>
-      <c r="AK2" s="70">
-        <v>8.5</v>
-      </c>
-      <c r="AL2" s="70">
-        <v>9</v>
-      </c>
-      <c r="AM2" s="70">
-        <v>9.5</v>
-      </c>
-      <c r="AN2" s="70">
+      <c r="AB2" s="161">
         <v>10</v>
       </c>
-      <c r="AO2" s="70">
-        <v>10.5</v>
-      </c>
-      <c r="AP2" s="70">
-        <v>11</v>
-      </c>
-      <c r="AQ2" s="70">
-        <v>11.5</v>
-      </c>
-      <c r="AR2" s="70">
+      <c r="AC2" s="161">
         <v>12</v>
       </c>
-      <c r="AS2" s="70">
-        <v>12.5</v>
-      </c>
-      <c r="AT2" s="70">
-        <v>13</v>
-      </c>
-      <c r="AU2" s="70">
-        <v>13.5</v>
-      </c>
-      <c r="AV2" s="70">
+      <c r="AD2" s="161">
         <v>14</v>
+      </c>
+      <c r="AE2" s="161">
+        <v>16</v>
+      </c>
+      <c r="AF2" s="161">
+        <v>20</v>
+      </c>
+      <c r="AG2" s="161">
+        <v>25</v>
+      </c>
+      <c r="AH2" s="161">
+        <v>30</v>
+      </c>
+      <c r="AI2" s="161">
+        <v>35</v>
+      </c>
+      <c r="AJ2" s="161">
+        <v>40</v>
+      </c>
+      <c r="AK2" s="161">
+        <v>45</v>
+      </c>
+      <c r="AL2" s="161">
+        <v>50</v>
+      </c>
+      <c r="AM2" s="161">
+        <v>55</v>
+      </c>
+      <c r="AN2" s="161">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="161">
+        <v>65</v>
+      </c>
+      <c r="AP2" s="161">
+        <v>70</v>
+      </c>
+      <c r="AQ2" s="161">
+        <v>75</v>
+      </c>
+      <c r="AR2" s="161">
+        <v>80</v>
+      </c>
+      <c r="AS2" s="161">
+        <v>100</v>
+      </c>
+      <c r="AT2" s="161">
+        <v>120</v>
+      </c>
+      <c r="AU2" s="161">
+        <v>140</v>
+      </c>
+      <c r="AV2" s="161">
+        <v>160</v>
       </c>
       <c r="AW2" s="70"/>
       <c r="AX2" s="70"/>

</xml_diff>